<commit_message>
a few edits before send out
</commit_message>
<xml_diff>
--- a/V2/Project Outputs for Badge_V2/Sources/BOM/PCB-00001-01_BOM-Badge_V2.xlsx
+++ b/V2/Project Outputs for Badge_V2/Sources/BOM/PCB-00001-01_BOM-Badge_V2.xlsx
@@ -1,15 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB4F220E-E499-4F7E-8147-98F25AF3D1BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradf\AppData\Local\TempReleases\Snapshot\1\Sources\BOM\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F51B9EC-4A60-479F-81CA-FC238B864D8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="18000" windowHeight="12675" xr2:uid="{F640D2EA-ACEC-410B-A5CC-23143916C43B}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{9EBB98DA-61C9-41A6-B07C-ABEBB5AAE766}"/>
   </bookViews>
   <sheets>
     <sheet name="PCB-00001-01_BOM-Badge_V2" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'PCB-00001-01_BOM-Badge_V2'!$1:$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
   <si>
     <t>Designator</t>
   </si>
@@ -61,6 +69,15 @@
   </si>
   <si>
     <t>CC0805JRNPO9BN330</t>
+  </si>
+  <si>
+    <t>GND, MISO, MOSI, SCK, VDD, VDD_CC</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Test Point</t>
   </si>
   <si>
     <t>LED1, LED2, LED3, LED4, LED5, LED6, LED7, LED8, LED9, LED10, LED11, LED12</t>
@@ -160,19 +177,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -184,7 +195,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="22"/>
+        <fgColor rgb="FFD3D3D3"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -216,13 +227,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,222 +552,239 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{103BA5FF-4490-4CF1-AC36-6AEA89FC3C0D}">
-  <dimension ref="A1:E12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD78A49C-03F9-40C7-82A3-36A24FD59EDC}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="14.42578125" customWidth="1"/>
+    <col min="1" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="4">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="4">
         <v>2</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="4">
+        <v>6</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="3">
+    </row>
+    <row r="5" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="4">
         <v>12</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="E5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="3">
+    </row>
+    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="4">
         <v>1</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="3">
+      <c r="E6" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4">
         <v>1</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="E7" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="3">
+      <c r="C8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="4">
         <v>13</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="E8" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="3">
+      <c r="C9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="4">
         <v>1</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="E9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="3">
+    </row>
+    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="4">
         <v>1</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="2" t="s">
+      <c r="E10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="3">
+    </row>
+    <row r="11" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="4">
         <v>1</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="E11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="3">
+    </row>
+    <row r="12" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="4">
         <v>1</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="2" t="s">
+      <c r="E12" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="3">
+    </row>
+    <row r="13" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="4">
         <v>1</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>41</v>
+      <c r="E13" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
+  <pageSetup orientation="landscape" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>